<commit_message>
button label from xlsx file
</commit_message>
<xml_diff>
--- a/database/Subject/Subject.xlsx
+++ b/database/Subject/Subject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saugau/Desktop/PROJECT/he_thong_tao_de_thi_cho_giao_vien/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saugau/Desktop/PROJECT/he_thong_tao_de_thi_cho_giao_vien/database/Subject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{643B2EB5-8DDF-384F-BB28-8A3305D9E53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527E307-0158-A44B-B801-D159224DB2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" xr2:uid="{1702D4EA-078E-474E-BB6A-E644CF4F9A88}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>